<commit_message>
Dead flotant model type update
-Model type for Dead_Flt changed from NullModel to NullModel_Coverage
</commit_message>
<xml_diff>
--- a/MP2023_LaVegMod3_Mortality_Tables.xlsx
+++ b/MP2023_LaVegMod3_Mortality_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\Documents\GitHub\ICM_LAVegMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{145B6909-E010-4B24-A4E3-8AF6A5073731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0C41FD-1BA9-4D48-A119-C00B9635E869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="1380" windowWidth="21600" windowHeight="11205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="28" r:id="rId1"/>
@@ -2234,9 +2234,9 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="4" width="11.42578125" style="37"/>
+    <col min="1" max="4" width="11.44140625" style="37"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2260,28 +2260,28 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.44140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="6" style="2" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" style="2" customWidth="1"/>
-    <col min="17" max="19" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="6.42578125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.7109375" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="2"/>
+    <col min="16" max="16" width="6.33203125" style="2" customWidth="1"/>
+    <col min="17" max="19" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.44140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="7.109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.6640625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -2314,7 +2314,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="39" t="s">
         <v>6</v>
@@ -4409,28 +4409,28 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.44140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="6" style="2" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" style="2" customWidth="1"/>
-    <col min="17" max="19" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="6.42578125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.7109375" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="2"/>
+    <col min="16" max="16" width="6.33203125" style="2" customWidth="1"/>
+    <col min="17" max="19" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.44140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="7.109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.6640625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -4463,7 +4463,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="39" t="s">
         <v>6</v>
@@ -6559,14 +6559,14 @@
       <selection sqref="A1:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="19" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="2"/>
+    <col min="1" max="1" width="3.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="19" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -6599,7 +6599,7 @@
       <c r="W1" s="203"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="15" thickBot="1">
+    <row r="2" spans="1:24" ht="14.4" thickBot="1">
       <c r="A2" s="202"/>
       <c r="B2" s="166" t="s">
         <v>145</v>
@@ -6668,7 +6668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="14.25">
+    <row r="3" spans="1:24" ht="13.8">
       <c r="A3" s="202"/>
       <c r="B3" s="172">
         <v>0</v>
@@ -6737,7 +6737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="14.25">
+    <row r="4" spans="1:24" ht="13.8">
       <c r="A4" s="202"/>
       <c r="B4" s="177">
         <v>0.2</v>
@@ -6806,7 +6806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="14.25">
+    <row r="5" spans="1:24" ht="13.8">
       <c r="A5" s="202"/>
       <c r="B5" s="180">
         <v>0.4</v>
@@ -6875,7 +6875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="14.25">
+    <row r="6" spans="1:24" ht="13.8">
       <c r="A6" s="202"/>
       <c r="B6" s="181">
         <v>0.6</v>
@@ -6944,7 +6944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="3" customFormat="1" ht="14.25">
+    <row r="7" spans="1:24" s="3" customFormat="1" ht="13.8">
       <c r="A7" s="202"/>
       <c r="B7" s="181">
         <v>0.8</v>
@@ -7013,7 +7013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="14.25">
+    <row r="8" spans="1:24" ht="13.8">
       <c r="A8" s="202"/>
       <c r="B8" s="182">
         <v>1</v>
@@ -7082,7 +7082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="14.25">
+    <row r="9" spans="1:24" ht="13.8">
       <c r="A9" s="202"/>
       <c r="B9" s="182">
         <v>1.2</v>
@@ -7151,7 +7151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="14.25">
+    <row r="10" spans="1:24" ht="13.8">
       <c r="A10" s="202"/>
       <c r="B10" s="182">
         <v>1.4</v>
@@ -7220,7 +7220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="14.25">
+    <row r="11" spans="1:24" ht="13.8">
       <c r="A11" s="202"/>
       <c r="B11" s="182">
         <v>1.6</v>
@@ -7289,7 +7289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="14.25">
+    <row r="12" spans="1:24" ht="13.8">
       <c r="A12" s="202"/>
       <c r="B12" s="182">
         <v>1.8</v>
@@ -7358,7 +7358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="14.25">
+    <row r="13" spans="1:24" ht="13.8">
       <c r="A13" s="202"/>
       <c r="B13" s="182">
         <v>2</v>
@@ -7427,7 +7427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="14.25">
+    <row r="14" spans="1:24" ht="13.8">
       <c r="A14" s="202"/>
       <c r="B14" s="182">
         <v>3</v>
@@ -7496,7 +7496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="14.25">
+    <row r="15" spans="1:24" ht="13.8">
       <c r="A15" s="202"/>
       <c r="B15" s="182">
         <v>4</v>
@@ -7565,7 +7565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="14.25">
+    <row r="16" spans="1:24" ht="13.8">
       <c r="A16" s="202"/>
       <c r="B16" s="182">
         <v>5</v>
@@ -7634,7 +7634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="14.25">
+    <row r="17" spans="1:23" ht="13.8">
       <c r="A17" s="202"/>
       <c r="B17" s="184">
         <v>6</v>
@@ -7703,7 +7703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="14.25">
+    <row r="18" spans="1:23" ht="13.8">
       <c r="A18" s="202"/>
       <c r="B18" s="184">
         <v>7</v>
@@ -7772,7 +7772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="14.25">
+    <row r="19" spans="1:23" ht="13.8">
       <c r="A19" s="202"/>
       <c r="B19" s="184">
         <v>8</v>
@@ -7841,7 +7841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="14.25">
+    <row r="20" spans="1:23" ht="13.8">
       <c r="A20" s="202"/>
       <c r="B20" s="184">
         <v>9</v>
@@ -7910,7 +7910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="14.25">
+    <row r="21" spans="1:23" ht="13.8">
       <c r="A21" s="202"/>
       <c r="B21" s="184">
         <v>10</v>
@@ -7979,7 +7979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="14.25">
+    <row r="22" spans="1:23" ht="13.8">
       <c r="A22" s="202"/>
       <c r="B22" s="184">
         <v>12</v>
@@ -8048,7 +8048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="14.25">
+    <row r="23" spans="1:23" ht="13.8">
       <c r="A23" s="202"/>
       <c r="B23" s="184">
         <v>14</v>
@@ -8117,7 +8117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="14.25">
+    <row r="24" spans="1:23" ht="13.8">
       <c r="A24" s="202"/>
       <c r="B24" s="184">
         <v>16</v>
@@ -8186,7 +8186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="14.25">
+    <row r="25" spans="1:23" ht="13.8">
       <c r="A25" s="202"/>
       <c r="B25" s="184">
         <v>18</v>
@@ -8255,7 +8255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="14.25">
+    <row r="26" spans="1:23" ht="13.8">
       <c r="A26" s="202"/>
       <c r="B26" s="184">
         <v>20</v>
@@ -8324,7 +8324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="14.25">
+    <row r="27" spans="1:23" ht="13.8">
       <c r="A27" s="202"/>
       <c r="B27" s="184">
         <v>22</v>
@@ -8393,7 +8393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="14.25">
+    <row r="28" spans="1:23" ht="13.8">
       <c r="A28" s="202"/>
       <c r="B28" s="184">
         <v>24</v>
@@ -8462,7 +8462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="14.25">
+    <row r="29" spans="1:23" ht="13.8">
       <c r="A29" s="202"/>
       <c r="B29" s="184">
         <v>26</v>
@@ -8531,7 +8531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="14.25">
+    <row r="30" spans="1:23" ht="13.8">
       <c r="A30" s="202"/>
       <c r="B30" s="184">
         <v>28</v>
@@ -8600,7 +8600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="14.25">
+    <row r="31" spans="1:23" ht="13.8">
       <c r="A31" s="202"/>
       <c r="B31" s="184">
         <v>100</v>
@@ -8690,16 +8690,16 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="19" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="6.42578125" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="2"/>
+    <col min="1" max="1" width="3.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="19" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="8.109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="6.44140625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -8732,7 +8732,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="76" t="s">
         <v>0</v>
@@ -10827,28 +10827,28 @@
       <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.44140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="6" style="2" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" style="2" customWidth="1"/>
-    <col min="17" max="19" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="6.42578125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.7109375" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="2"/>
+    <col min="16" max="16" width="6.33203125" style="2" customWidth="1"/>
+    <col min="17" max="19" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.44140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="7.109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.6640625" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -10881,7 +10881,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="39" t="s">
         <v>6</v>
@@ -12977,16 +12977,16 @@
       <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="22" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="3"/>
+    <col min="24" max="16384" width="5.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -13019,7 +13019,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="75" t="s">
         <v>46</v>
@@ -13088,7 +13088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="12.95" customHeight="1">
+    <row r="3" spans="1:24" ht="12.9" customHeight="1">
       <c r="A3" s="198"/>
       <c r="B3" s="12">
         <v>0</v>
@@ -13157,7 +13157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="12.95" customHeight="1">
+    <row r="4" spans="1:24" ht="12.9" customHeight="1">
       <c r="A4" s="198"/>
       <c r="B4" s="24">
         <v>0.2</v>
@@ -13226,7 +13226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="12.95" customHeight="1">
+    <row r="5" spans="1:24" ht="12.9" customHeight="1">
       <c r="A5" s="198"/>
       <c r="B5" s="26">
         <v>0.4</v>
@@ -13295,7 +13295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="12.95" customHeight="1">
+    <row r="6" spans="1:24" ht="12.9" customHeight="1">
       <c r="A6" s="198"/>
       <c r="B6" s="26">
         <v>0.6</v>
@@ -13364,7 +13364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="12.95" customHeight="1">
+    <row r="7" spans="1:24" ht="12.9" customHeight="1">
       <c r="A7" s="198"/>
       <c r="B7" s="14">
         <v>0.8</v>
@@ -13433,7 +13433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="12.95" customHeight="1">
+    <row r="8" spans="1:24" ht="12.9" customHeight="1">
       <c r="A8" s="198"/>
       <c r="B8" s="14">
         <v>1</v>
@@ -13502,7 +13502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="12.95" customHeight="1">
+    <row r="9" spans="1:24" ht="12.9" customHeight="1">
       <c r="A9" s="198"/>
       <c r="B9" s="14">
         <v>1.2</v>
@@ -13571,7 +13571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="12.95" customHeight="1">
+    <row r="10" spans="1:24" ht="12.9" customHeight="1">
       <c r="A10" s="198"/>
       <c r="B10" s="14">
         <v>1.4</v>
@@ -13640,7 +13640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="12.95" customHeight="1">
+    <row r="11" spans="1:24" ht="12.9" customHeight="1">
       <c r="A11" s="198"/>
       <c r="B11" s="14">
         <v>1.6</v>
@@ -13709,7 +13709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="12.95" customHeight="1">
+    <row r="12" spans="1:24" ht="12.9" customHeight="1">
       <c r="A12" s="198"/>
       <c r="B12" s="12">
         <v>1.8</v>
@@ -13778,7 +13778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="12.95" customHeight="1">
+    <row r="13" spans="1:24" ht="12.9" customHeight="1">
       <c r="A13" s="198"/>
       <c r="B13" s="12">
         <v>2</v>
@@ -13847,7 +13847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="12.95" customHeight="1">
+    <row r="14" spans="1:24" ht="12.9" customHeight="1">
       <c r="A14" s="198"/>
       <c r="B14" s="12">
         <v>3</v>
@@ -13916,7 +13916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="12.95" customHeight="1">
+    <row r="15" spans="1:24" ht="12.9" customHeight="1">
       <c r="A15" s="198"/>
       <c r="B15" s="12">
         <v>4</v>
@@ -13985,7 +13985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="12.95" customHeight="1">
+    <row r="16" spans="1:24" ht="12.9" customHeight="1">
       <c r="A16" s="198"/>
       <c r="B16" s="12">
         <v>5</v>
@@ -14054,7 +14054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="12.95" customHeight="1">
+    <row r="17" spans="1:23" ht="12.9" customHeight="1">
       <c r="A17" s="198"/>
       <c r="B17" s="12">
         <v>6</v>
@@ -14123,7 +14123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="12.95" customHeight="1">
+    <row r="18" spans="1:23" ht="12.9" customHeight="1">
       <c r="A18" s="198"/>
       <c r="B18" s="12">
         <v>7</v>
@@ -14192,7 +14192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="12.95" customHeight="1">
+    <row r="19" spans="1:23" ht="12.9" customHeight="1">
       <c r="A19" s="198"/>
       <c r="B19" s="12">
         <v>8</v>
@@ -14261,7 +14261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="12.95" customHeight="1">
+    <row r="20" spans="1:23" ht="12.9" customHeight="1">
       <c r="A20" s="198"/>
       <c r="B20" s="12">
         <v>9</v>
@@ -14330,7 +14330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="12.95" customHeight="1">
+    <row r="21" spans="1:23" ht="12.9" customHeight="1">
       <c r="A21" s="198"/>
       <c r="B21" s="12">
         <v>10</v>
@@ -14399,7 +14399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="12.95" customHeight="1">
+    <row r="22" spans="1:23" ht="12.9" customHeight="1">
       <c r="A22" s="198"/>
       <c r="B22" s="12">
         <v>12</v>
@@ -14468,7 +14468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="12.95" customHeight="1">
+    <row r="23" spans="1:23" ht="12.9" customHeight="1">
       <c r="A23" s="198"/>
       <c r="B23" s="12">
         <v>14</v>
@@ -14537,7 +14537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="12.95" customHeight="1">
+    <row r="24" spans="1:23" ht="12.9" customHeight="1">
       <c r="A24" s="198"/>
       <c r="B24" s="12">
         <v>16</v>
@@ -14606,7 +14606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="12.95" customHeight="1">
+    <row r="25" spans="1:23" ht="12.9" customHeight="1">
       <c r="A25" s="198"/>
       <c r="B25" s="12">
         <v>18</v>
@@ -14675,7 +14675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="12.95" customHeight="1">
+    <row r="26" spans="1:23" ht="12.9" customHeight="1">
       <c r="A26" s="198"/>
       <c r="B26" s="12">
         <v>20</v>
@@ -14744,7 +14744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="12.95" customHeight="1">
+    <row r="27" spans="1:23" ht="12.9" customHeight="1">
       <c r="A27" s="198"/>
       <c r="B27" s="12">
         <v>22</v>
@@ -14813,7 +14813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="12.95" customHeight="1">
+    <row r="28" spans="1:23" ht="12.9" customHeight="1">
       <c r="A28" s="198"/>
       <c r="B28" s="12">
         <v>24</v>
@@ -14882,7 +14882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="12.95" customHeight="1">
+    <row r="29" spans="1:23" ht="12.9" customHeight="1">
       <c r="A29" s="198"/>
       <c r="B29" s="12">
         <v>26</v>
@@ -14951,7 +14951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="12.95" customHeight="1">
+    <row r="30" spans="1:23" ht="12.9" customHeight="1">
       <c r="A30" s="198"/>
       <c r="B30" s="12">
         <v>28</v>
@@ -15020,7 +15020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="12.95" customHeight="1">
+    <row r="31" spans="1:23" ht="12.9" customHeight="1">
       <c r="A31" s="198"/>
       <c r="B31" s="12">
         <v>100</v>
@@ -15115,13 +15115,13 @@
       <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="23" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="3"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="23" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -15154,7 +15154,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="41" t="s">
         <v>3</v>
@@ -15223,7 +15223,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="12.95" customHeight="1">
+    <row r="3" spans="1:24" ht="12.9" customHeight="1">
       <c r="A3" s="198"/>
       <c r="B3" s="12">
         <v>0</v>
@@ -15292,7 +15292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="12.95" customHeight="1">
+    <row r="4" spans="1:24" ht="12.9" customHeight="1">
       <c r="A4" s="198"/>
       <c r="B4" s="24">
         <v>0.2</v>
@@ -15361,7 +15361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="12.95" customHeight="1">
+    <row r="5" spans="1:24" ht="12.9" customHeight="1">
       <c r="A5" s="198"/>
       <c r="B5" s="26">
         <v>0.4</v>
@@ -15430,7 +15430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="12.95" customHeight="1">
+    <row r="6" spans="1:24" ht="12.9" customHeight="1">
       <c r="A6" s="198"/>
       <c r="B6" s="26">
         <v>0.6</v>
@@ -15499,7 +15499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="12.95" customHeight="1">
+    <row r="7" spans="1:24" ht="12.9" customHeight="1">
       <c r="A7" s="198"/>
       <c r="B7" s="26">
         <v>0.8</v>
@@ -15568,7 +15568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="12.95" customHeight="1">
+    <row r="8" spans="1:24" ht="12.9" customHeight="1">
       <c r="A8" s="198"/>
       <c r="B8" s="14">
         <v>1</v>
@@ -15637,7 +15637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="12.95" customHeight="1">
+    <row r="9" spans="1:24" ht="12.9" customHeight="1">
       <c r="A9" s="198"/>
       <c r="B9" s="14">
         <v>1.2</v>
@@ -15706,7 +15706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="12.95" customHeight="1">
+    <row r="10" spans="1:24" ht="12.9" customHeight="1">
       <c r="A10" s="198"/>
       <c r="B10" s="14">
         <v>1.4</v>
@@ -15775,7 +15775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="12.95" customHeight="1">
+    <row r="11" spans="1:24" ht="12.9" customHeight="1">
       <c r="A11" s="198"/>
       <c r="B11" s="14">
         <v>1.6</v>
@@ -15844,7 +15844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="12.95" customHeight="1">
+    <row r="12" spans="1:24" ht="12.9" customHeight="1">
       <c r="A12" s="198"/>
       <c r="B12" s="14">
         <v>1.8</v>
@@ -15913,7 +15913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="12.95" customHeight="1">
+    <row r="13" spans="1:24" ht="12.9" customHeight="1">
       <c r="A13" s="198"/>
       <c r="B13" s="12">
         <v>2</v>
@@ -15982,7 +15982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="12.95" customHeight="1">
+    <row r="14" spans="1:24" ht="12.9" customHeight="1">
       <c r="A14" s="198"/>
       <c r="B14" s="12">
         <v>3</v>
@@ -16051,7 +16051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="12.95" customHeight="1">
+    <row r="15" spans="1:24" ht="12.9" customHeight="1">
       <c r="A15" s="198"/>
       <c r="B15" s="12">
         <v>4</v>
@@ -16120,7 +16120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="12.95" customHeight="1">
+    <row r="16" spans="1:24" ht="12.9" customHeight="1">
       <c r="A16" s="198"/>
       <c r="B16" s="12">
         <v>5</v>
@@ -16189,7 +16189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="12.95" customHeight="1">
+    <row r="17" spans="1:23" ht="12.9" customHeight="1">
       <c r="A17" s="198"/>
       <c r="B17" s="12">
         <v>6</v>
@@ -16258,7 +16258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="12.95" customHeight="1">
+    <row r="18" spans="1:23" ht="12.9" customHeight="1">
       <c r="A18" s="198"/>
       <c r="B18" s="12">
         <v>7</v>
@@ -16327,7 +16327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="12.95" customHeight="1">
+    <row r="19" spans="1:23" ht="12.9" customHeight="1">
       <c r="A19" s="198"/>
       <c r="B19" s="12">
         <v>8</v>
@@ -16396,7 +16396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="12.95" customHeight="1">
+    <row r="20" spans="1:23" ht="12.9" customHeight="1">
       <c r="A20" s="198"/>
       <c r="B20" s="12">
         <v>9</v>
@@ -16465,7 +16465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="12.95" customHeight="1">
+    <row r="21" spans="1:23" ht="12.9" customHeight="1">
       <c r="A21" s="198"/>
       <c r="B21" s="12">
         <v>10</v>
@@ -16534,7 +16534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="12.95" customHeight="1">
+    <row r="22" spans="1:23" ht="12.9" customHeight="1">
       <c r="A22" s="198"/>
       <c r="B22" s="12">
         <v>12</v>
@@ -16603,7 +16603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="12.95" customHeight="1">
+    <row r="23" spans="1:23" ht="12.9" customHeight="1">
       <c r="A23" s="198"/>
       <c r="B23" s="12">
         <v>14</v>
@@ -16672,7 +16672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="12.95" customHeight="1">
+    <row r="24" spans="1:23" ht="12.9" customHeight="1">
       <c r="A24" s="198"/>
       <c r="B24" s="12">
         <v>16</v>
@@ -16741,7 +16741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="12.95" customHeight="1">
+    <row r="25" spans="1:23" ht="12.9" customHeight="1">
       <c r="A25" s="198"/>
       <c r="B25" s="12">
         <v>18</v>
@@ -16810,7 +16810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="12.95" customHeight="1">
+    <row r="26" spans="1:23" ht="12.9" customHeight="1">
       <c r="A26" s="198"/>
       <c r="B26" s="12">
         <v>20</v>
@@ -16879,7 +16879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="12.95" customHeight="1">
+    <row r="27" spans="1:23" ht="12.9" customHeight="1">
       <c r="A27" s="198"/>
       <c r="B27" s="12">
         <v>22</v>
@@ -16948,7 +16948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="12.95" customHeight="1">
+    <row r="28" spans="1:23" ht="12.9" customHeight="1">
       <c r="A28" s="198"/>
       <c r="B28" s="12">
         <v>24</v>
@@ -17017,7 +17017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="12.95" customHeight="1">
+    <row r="29" spans="1:23" ht="12.9" customHeight="1">
       <c r="A29" s="198"/>
       <c r="B29" s="12">
         <v>26</v>
@@ -17086,7 +17086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="12.95" customHeight="1">
+    <row r="30" spans="1:23" ht="12.9" customHeight="1">
       <c r="A30" s="198"/>
       <c r="B30" s="12">
         <v>28</v>
@@ -17155,7 +17155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="12.95" customHeight="1">
+    <row r="31" spans="1:23" ht="12.9" customHeight="1">
       <c r="A31" s="198"/>
       <c r="B31" s="12">
         <v>100</v>
@@ -17251,16 +17251,16 @@
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" style="3" customWidth="1"/>
     <col min="9" max="22" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="3"/>
+    <col min="24" max="16384" width="5.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -17293,7 +17293,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="38" t="s">
         <v>21</v>
@@ -19390,16 +19390,16 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="3" customWidth="1"/>
-    <col min="9" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="3"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" style="3" customWidth="1"/>
+    <col min="9" max="22" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -19432,7 +19432,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="38" t="s">
         <v>148</v>
@@ -21523,16 +21523,16 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="3" customWidth="1"/>
-    <col min="9" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="3"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" style="3" customWidth="1"/>
+    <col min="9" max="22" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="16" customFormat="1" ht="18" customHeight="1">
@@ -21565,7 +21565,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:32" ht="13.5" thickBot="1">
+    <row r="2" spans="1:32" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="38" t="s">
         <v>143</v>
@@ -21841,7 +21841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="15">
+    <row r="6" spans="1:32" ht="14.4">
       <c r="A6" s="198"/>
       <c r="B6" s="26">
         <v>0.6</v>
@@ -21911,7 +21911,7 @@
       </c>
       <c r="AF6" s="163"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75">
+    <row r="7" spans="1:32" ht="15.6">
       <c r="A7" s="198"/>
       <c r="B7" s="26">
         <v>0.8</v>
@@ -21981,7 +21981,7 @@
       </c>
       <c r="AF7" s="53"/>
     </row>
-    <row r="8" spans="1:32" ht="15">
+    <row r="8" spans="1:32" ht="14.4">
       <c r="A8" s="198"/>
       <c r="B8" s="34">
         <v>1</v>
@@ -22051,7 +22051,7 @@
       </c>
       <c r="AF8" s="163"/>
     </row>
-    <row r="9" spans="1:32" ht="15">
+    <row r="9" spans="1:32" ht="14.4">
       <c r="A9" s="198"/>
       <c r="B9" s="34">
         <v>1.2</v>
@@ -22121,7 +22121,7 @@
       </c>
       <c r="AF9" s="163"/>
     </row>
-    <row r="10" spans="1:32" ht="15">
+    <row r="10" spans="1:32" ht="14.4">
       <c r="A10" s="198"/>
       <c r="B10" s="34">
         <v>1.4</v>
@@ -22191,7 +22191,7 @@
       </c>
       <c r="AF10" s="163"/>
     </row>
-    <row r="11" spans="1:32" ht="15">
+    <row r="11" spans="1:32" ht="14.4">
       <c r="A11" s="198"/>
       <c r="B11" s="34">
         <v>1.6</v>
@@ -22261,7 +22261,7 @@
       </c>
       <c r="AF11" s="163"/>
     </row>
-    <row r="12" spans="1:32" ht="15">
+    <row r="12" spans="1:32" ht="14.4">
       <c r="A12" s="198"/>
       <c r="B12" s="34">
         <v>1.8</v>
@@ -22331,7 +22331,7 @@
       </c>
       <c r="AF12" s="163"/>
     </row>
-    <row r="13" spans="1:32" ht="15.75">
+    <row r="13" spans="1:32" ht="15.6">
       <c r="A13" s="198"/>
       <c r="B13" s="34">
         <v>2</v>
@@ -22401,7 +22401,7 @@
       </c>
       <c r="AF13" s="56"/>
     </row>
-    <row r="14" spans="1:32" ht="15.75">
+    <row r="14" spans="1:32" ht="15.6">
       <c r="A14" s="198"/>
       <c r="B14" s="34">
         <v>3</v>
@@ -22471,7 +22471,7 @@
       </c>
       <c r="AF14" s="56"/>
     </row>
-    <row r="15" spans="1:32" ht="15">
+    <row r="15" spans="1:32" ht="14.4">
       <c r="A15" s="198"/>
       <c r="B15" s="12">
         <v>4</v>
@@ -22541,7 +22541,7 @@
       </c>
       <c r="AF15" s="163"/>
     </row>
-    <row r="16" spans="1:32" ht="15">
+    <row r="16" spans="1:32" ht="14.4">
       <c r="A16" s="198"/>
       <c r="B16" s="12">
         <v>5</v>
@@ -22611,7 +22611,7 @@
       </c>
       <c r="AF16" s="163"/>
     </row>
-    <row r="17" spans="1:32" ht="15">
+    <row r="17" spans="1:32" ht="14.4">
       <c r="A17" s="198"/>
       <c r="B17" s="12">
         <v>6</v>
@@ -22681,7 +22681,7 @@
       </c>
       <c r="AF17" s="163"/>
     </row>
-    <row r="18" spans="1:32" ht="15">
+    <row r="18" spans="1:32" ht="14.4">
       <c r="A18" s="198"/>
       <c r="B18" s="12">
         <v>7</v>
@@ -22751,7 +22751,7 @@
       </c>
       <c r="AF18" s="163"/>
     </row>
-    <row r="19" spans="1:32" ht="15">
+    <row r="19" spans="1:32" ht="14.4">
       <c r="A19" s="198"/>
       <c r="B19" s="12">
         <v>8</v>
@@ -23665,19 +23665,19 @@
   <dimension ref="A1:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" style="160" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="160" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="160" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="160" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="160" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="160" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="160" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="160" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" style="160" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="160" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="160" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11.5703125" style="160" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" style="160" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="160" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.5546875" style="160" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="162" customFormat="1">
@@ -24208,7 +24208,7 @@
         <v>135</v>
       </c>
       <c r="D18" s="160" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
       <c r="E18" s="160" t="s">
         <v>135</v>
@@ -25247,17 +25247,17 @@
       <selection activeCell="AA46" sqref="AA46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="22" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -25290,7 +25290,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="43" t="s">
         <v>12</v>
@@ -27387,11 +27387,11 @@
       <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -27424,7 +27424,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="16.5" thickBot="1">
+    <row r="2" spans="1:24" ht="16.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="45" t="s">
         <v>14</v>
@@ -29520,15 +29520,15 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="1" max="1" width="3.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -29561,7 +29561,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="46" t="s">
         <v>16</v>
@@ -31657,18 +31657,18 @@
       <selection activeCell="AC50" sqref="AC50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="22" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="3" max="3" width="2.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="22" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -31701,7 +31701,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="42" t="s">
         <v>11</v>
@@ -33797,12 +33797,12 @@
       <selection activeCell="X48" sqref="X48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -33835,7 +33835,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="44" t="s">
         <v>10</v>
@@ -35931,13 +35931,13 @@
       <selection activeCell="AD42" sqref="AD42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="3"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="22" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -35970,7 +35970,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="40" t="s">
         <v>9</v>
@@ -38084,16 +38084,16 @@
       <selection sqref="A1:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="9" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="16" customFormat="1" ht="18" customHeight="1">
@@ -38126,7 +38126,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:31" ht="13.5" thickBot="1">
+    <row r="2" spans="1:31" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="77" t="s">
         <v>139</v>
@@ -38195,7 +38195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15">
+    <row r="3" spans="1:31" ht="14.4">
       <c r="A3" s="198"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -38265,7 +38265,7 @@
       </c>
       <c r="AE3" s="163"/>
     </row>
-    <row r="4" spans="1:31" ht="15.75">
+    <row r="4" spans="1:31" ht="15.6">
       <c r="A4" s="198"/>
       <c r="B4" s="8">
         <v>0.2</v>
@@ -38335,7 +38335,7 @@
       </c>
       <c r="AE4" s="53"/>
     </row>
-    <row r="5" spans="1:31" ht="15">
+    <row r="5" spans="1:31" ht="14.4">
       <c r="A5" s="198"/>
       <c r="B5" s="34">
         <v>0.4</v>
@@ -38405,7 +38405,7 @@
       </c>
       <c r="AE5" s="163"/>
     </row>
-    <row r="6" spans="1:31" ht="15">
+    <row r="6" spans="1:31" ht="14.4">
       <c r="A6" s="198"/>
       <c r="B6" s="34">
         <v>0.6</v>
@@ -38475,7 +38475,7 @@
       </c>
       <c r="AE6" s="163"/>
     </row>
-    <row r="7" spans="1:31" ht="15">
+    <row r="7" spans="1:31" ht="14.4">
       <c r="A7" s="198"/>
       <c r="B7" s="34">
         <v>0.8</v>
@@ -38545,7 +38545,7 @@
       </c>
       <c r="AE7" s="163"/>
     </row>
-    <row r="8" spans="1:31" ht="15">
+    <row r="8" spans="1:31" ht="14.4">
       <c r="A8" s="198"/>
       <c r="B8" s="34">
         <v>1</v>
@@ -38615,7 +38615,7 @@
       </c>
       <c r="AE8" s="163"/>
     </row>
-    <row r="9" spans="1:31" ht="15">
+    <row r="9" spans="1:31" ht="14.4">
       <c r="A9" s="198"/>
       <c r="B9" s="34">
         <v>1.2</v>
@@ -38685,7 +38685,7 @@
       </c>
       <c r="AE9" s="163"/>
     </row>
-    <row r="10" spans="1:31" ht="15.75">
+    <row r="10" spans="1:31" ht="15.6">
       <c r="A10" s="198"/>
       <c r="B10" s="34">
         <v>1.4</v>
@@ -38755,7 +38755,7 @@
       </c>
       <c r="AE10" s="56"/>
     </row>
-    <row r="11" spans="1:31" ht="15.75">
+    <row r="11" spans="1:31" ht="15.6">
       <c r="A11" s="198"/>
       <c r="B11" s="26">
         <v>1.6</v>
@@ -38825,7 +38825,7 @@
       </c>
       <c r="AE11" s="56"/>
     </row>
-    <row r="12" spans="1:31" ht="15">
+    <row r="12" spans="1:31" ht="14.4">
       <c r="A12" s="198"/>
       <c r="B12" s="26">
         <v>1.8</v>
@@ -38895,7 +38895,7 @@
       </c>
       <c r="AE12" s="163"/>
     </row>
-    <row r="13" spans="1:31" ht="15">
+    <row r="13" spans="1:31" ht="14.4">
       <c r="A13" s="198"/>
       <c r="B13" s="26">
         <v>2</v>
@@ -38965,7 +38965,7 @@
       </c>
       <c r="AE13" s="163"/>
     </row>
-    <row r="14" spans="1:31" ht="15">
+    <row r="14" spans="1:31" ht="14.4">
       <c r="A14" s="198"/>
       <c r="B14" s="26">
         <v>3</v>
@@ -39035,7 +39035,7 @@
       </c>
       <c r="AE14" s="163"/>
     </row>
-    <row r="15" spans="1:31" ht="15">
+    <row r="15" spans="1:31" ht="14.4">
       <c r="A15" s="198"/>
       <c r="B15" s="24">
         <v>4</v>
@@ -39105,7 +39105,7 @@
       </c>
       <c r="AE15" s="163"/>
     </row>
-    <row r="16" spans="1:31" ht="15">
+    <row r="16" spans="1:31" ht="14.4">
       <c r="A16" s="198"/>
       <c r="B16" s="26">
         <v>5</v>
@@ -40230,16 +40230,16 @@
       <selection sqref="A1:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="9" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="16" customFormat="1" ht="18" customHeight="1">
@@ -40272,7 +40272,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" thickBot="1">
+    <row r="2" spans="1:28" ht="15" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="77" t="s">
         <v>150</v>
@@ -40342,7 +40342,7 @@
       </c>
       <c r="AB2" s="163"/>
     </row>
-    <row r="3" spans="1:28" ht="15.75">
+    <row r="3" spans="1:28" ht="15.6">
       <c r="A3" s="198"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -40412,7 +40412,7 @@
       </c>
       <c r="AB3" s="53"/>
     </row>
-    <row r="4" spans="1:28" ht="15">
+    <row r="4" spans="1:28" ht="14.4">
       <c r="A4" s="198"/>
       <c r="B4" s="8">
         <v>0.2</v>
@@ -40482,7 +40482,7 @@
       </c>
       <c r="AB4" s="163"/>
     </row>
-    <row r="5" spans="1:28" ht="15">
+    <row r="5" spans="1:28" ht="14.4">
       <c r="A5" s="198"/>
       <c r="B5" s="8">
         <v>0.4</v>
@@ -40552,7 +40552,7 @@
       </c>
       <c r="AB5" s="163"/>
     </row>
-    <row r="6" spans="1:28" ht="15">
+    <row r="6" spans="1:28" ht="14.4">
       <c r="A6" s="198"/>
       <c r="B6" s="8">
         <v>0.6</v>
@@ -40622,7 +40622,7 @@
       </c>
       <c r="AB6" s="163"/>
     </row>
-    <row r="7" spans="1:28" ht="15">
+    <row r="7" spans="1:28" ht="14.4">
       <c r="A7" s="198"/>
       <c r="B7" s="8">
         <v>0.8</v>
@@ -40692,7 +40692,7 @@
       </c>
       <c r="AB7" s="163"/>
     </row>
-    <row r="8" spans="1:28" ht="15">
+    <row r="8" spans="1:28" ht="14.4">
       <c r="A8" s="198"/>
       <c r="B8" s="8">
         <v>1</v>
@@ -40762,7 +40762,7 @@
       </c>
       <c r="AB8" s="163"/>
     </row>
-    <row r="9" spans="1:28" ht="15.75">
+    <row r="9" spans="1:28" ht="15.6">
       <c r="A9" s="198"/>
       <c r="B9" s="8">
         <v>1.2</v>
@@ -40832,7 +40832,7 @@
       </c>
       <c r="AB9" s="56"/>
     </row>
-    <row r="10" spans="1:28" ht="15.75">
+    <row r="10" spans="1:28" ht="15.6">
       <c r="A10" s="198"/>
       <c r="B10" s="8">
         <v>1.4</v>
@@ -40902,7 +40902,7 @@
       </c>
       <c r="AB10" s="56"/>
     </row>
-    <row r="11" spans="1:28" ht="15">
+    <row r="11" spans="1:28" ht="14.4">
       <c r="A11" s="198"/>
       <c r="B11" s="34">
         <v>1.6</v>
@@ -40972,7 +40972,7 @@
       </c>
       <c r="AB11" s="163"/>
     </row>
-    <row r="12" spans="1:28" ht="15">
+    <row r="12" spans="1:28" ht="14.4">
       <c r="A12" s="198"/>
       <c r="B12" s="34">
         <v>1.8</v>
@@ -41042,7 +41042,7 @@
       </c>
       <c r="AB12" s="163"/>
     </row>
-    <row r="13" spans="1:28" ht="15">
+    <row r="13" spans="1:28" ht="14.4">
       <c r="A13" s="198"/>
       <c r="B13" s="34">
         <v>2</v>
@@ -41112,7 +41112,7 @@
       </c>
       <c r="AB13" s="163"/>
     </row>
-    <row r="14" spans="1:28" ht="15">
+    <row r="14" spans="1:28" ht="14.4">
       <c r="A14" s="198"/>
       <c r="B14" s="26">
         <v>3</v>
@@ -41182,7 +41182,7 @@
       </c>
       <c r="AB14" s="163"/>
     </row>
-    <row r="15" spans="1:28" ht="15">
+    <row r="15" spans="1:28" ht="14.4">
       <c r="A15" s="198"/>
       <c r="B15" s="26">
         <v>4</v>
@@ -42376,15 +42376,15 @@
       <selection activeCell="B2" sqref="B2:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.6640625" style="1" customWidth="1"/>
+    <col min="5" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="9" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -42417,7 +42417,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="77" t="s">
         <v>15</v>
@@ -44512,16 +44512,16 @@
       <selection sqref="A1:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="9" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="16" customFormat="1" ht="18" customHeight="1">
@@ -44554,7 +44554,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" thickBot="1">
+    <row r="2" spans="1:28" ht="15" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="77" t="s">
         <v>141</v>
@@ -44624,7 +44624,7 @@
       </c>
       <c r="AB2" s="163"/>
     </row>
-    <row r="3" spans="1:28" ht="15.75">
+    <row r="3" spans="1:28" ht="15.6">
       <c r="A3" s="198"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -44694,7 +44694,7 @@
       </c>
       <c r="AB3" s="53"/>
     </row>
-    <row r="4" spans="1:28" ht="15">
+    <row r="4" spans="1:28" ht="14.4">
       <c r="A4" s="198"/>
       <c r="B4" s="8">
         <v>0.2</v>
@@ -44764,7 +44764,7 @@
       </c>
       <c r="AB4" s="163"/>
     </row>
-    <row r="5" spans="1:28" ht="15">
+    <row r="5" spans="1:28" ht="14.4">
       <c r="A5" s="198"/>
       <c r="B5" s="8">
         <v>0.4</v>
@@ -44834,7 +44834,7 @@
       </c>
       <c r="AB5" s="163"/>
     </row>
-    <row r="6" spans="1:28" ht="15">
+    <row r="6" spans="1:28" ht="14.4">
       <c r="A6" s="198"/>
       <c r="B6" s="8">
         <v>0.6</v>
@@ -44904,7 +44904,7 @@
       </c>
       <c r="AB6" s="163"/>
     </row>
-    <row r="7" spans="1:28" ht="15">
+    <row r="7" spans="1:28" ht="14.4">
       <c r="A7" s="198"/>
       <c r="B7" s="34">
         <v>0.8</v>
@@ -44974,7 +44974,7 @@
       </c>
       <c r="AB7" s="163"/>
     </row>
-    <row r="8" spans="1:28" ht="15">
+    <row r="8" spans="1:28" ht="14.4">
       <c r="A8" s="198"/>
       <c r="B8" s="34">
         <v>1</v>
@@ -45044,7 +45044,7 @@
       </c>
       <c r="AB8" s="163"/>
     </row>
-    <row r="9" spans="1:28" ht="15.75">
+    <row r="9" spans="1:28" ht="15.6">
       <c r="A9" s="198"/>
       <c r="B9" s="34">
         <v>1.2</v>
@@ -45114,7 +45114,7 @@
       </c>
       <c r="AB9" s="56"/>
     </row>
-    <row r="10" spans="1:28" ht="15.75">
+    <row r="10" spans="1:28" ht="15.6">
       <c r="A10" s="198"/>
       <c r="B10" s="34">
         <v>1.4</v>
@@ -45184,7 +45184,7 @@
       </c>
       <c r="AB10" s="56"/>
     </row>
-    <row r="11" spans="1:28" ht="15">
+    <row r="11" spans="1:28" ht="14.4">
       <c r="A11" s="198"/>
       <c r="B11" s="34">
         <v>1.6</v>
@@ -45254,7 +45254,7 @@
       </c>
       <c r="AB11" s="163"/>
     </row>
-    <row r="12" spans="1:28" ht="15">
+    <row r="12" spans="1:28" ht="14.4">
       <c r="A12" s="198"/>
       <c r="B12" s="34">
         <v>1.8</v>
@@ -45324,7 +45324,7 @@
       </c>
       <c r="AB12" s="163"/>
     </row>
-    <row r="13" spans="1:28" ht="15">
+    <row r="13" spans="1:28" ht="14.4">
       <c r="A13" s="198"/>
       <c r="B13" s="26">
         <v>2</v>
@@ -45394,7 +45394,7 @@
       </c>
       <c r="AB13" s="163"/>
     </row>
-    <row r="14" spans="1:28" ht="15">
+    <row r="14" spans="1:28" ht="14.4">
       <c r="A14" s="198"/>
       <c r="B14" s="26">
         <v>3</v>
@@ -45464,7 +45464,7 @@
       </c>
       <c r="AB14" s="163"/>
     </row>
-    <row r="15" spans="1:28" ht="15">
+    <row r="15" spans="1:28" ht="14.4">
       <c r="A15" s="198"/>
       <c r="B15" s="24">
         <v>4</v>
@@ -46657,41 +46657,41 @@
       <selection pane="topRight" activeCell="AL9" sqref="AL9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="13" style="52" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="52" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="52" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="64" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" style="64" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" style="52" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="52" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="52" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.88671875" style="52" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8" style="52" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="8.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="30" max="34" width="10.7109375" style="52" customWidth="1"/>
-    <col min="35" max="16384" width="10.85546875" style="52"/>
+    <col min="26" max="26" width="9.109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="8.109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="10.6640625" style="52" customWidth="1"/>
+    <col min="35" max="16384" width="10.88671875" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="31.5">
+    <row r="1" spans="1:35" ht="31.2">
       <c r="A1" s="51" t="s">
         <v>22</v>
       </c>
@@ -46798,7 +46798,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="53" customFormat="1" ht="31.5">
+    <row r="2" spans="1:35" s="53" customFormat="1" ht="31.2">
       <c r="A2" s="49" t="s">
         <v>23</v>
       </c>
@@ -48272,15 +48272,15 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -48313,7 +48313,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="78" t="s">
         <v>18</v>
@@ -50408,14 +50408,14 @@
       <selection activeCell="Y46" sqref="Y46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="3" max="17" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -50448,7 +50448,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="47" t="s">
         <v>17</v>
@@ -52543,17 +52543,17 @@
       <selection activeCell="AA52" sqref="AA52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="1" customWidth="1"/>
     <col min="4" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="17" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -52586,7 +52586,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="48" t="s">
         <v>20</v>
@@ -54242,7 +54242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="13.5" thickBot="1">
+    <row r="26" spans="1:23" ht="13.2" thickBot="1">
       <c r="A26" s="198"/>
       <c r="B26" s="11">
         <v>20</v>
@@ -54311,7 +54311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="13.5" thickTop="1">
+    <row r="27" spans="1:23" ht="13.2" thickTop="1">
       <c r="A27" s="198"/>
       <c r="B27" s="143">
         <v>22</v>
@@ -54587,7 +54587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="13.5" thickBot="1">
+    <row r="31" spans="1:23" ht="13.2" thickBot="1">
       <c r="A31" s="198"/>
       <c r="B31" s="145">
         <v>30</v>
@@ -54656,7 +54656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="13.5" thickTop="1">
+    <row r="32" spans="1:23" ht="13.2" thickTop="1">
       <c r="B32" s="1">
         <v>35</v>
       </c>
@@ -54955,13 +54955,13 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="116" bestFit="1" customWidth="1"/>
-    <col min="3" max="22" width="4.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="1"/>
+    <col min="1" max="1" width="4.88671875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="116" bestFit="1" customWidth="1"/>
+    <col min="3" max="22" width="4.88671875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.109375" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -54994,7 +54994,7 @@
       <c r="W1" s="204"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="205"/>
       <c r="B2" s="113" t="s">
         <v>19</v>
@@ -56029,7 +56029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="13.5" thickBot="1">
+    <row r="17" spans="1:23" ht="13.2" thickBot="1">
       <c r="A17" s="205"/>
       <c r="B17" s="115">
         <v>6</v>
@@ -56098,7 +56098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="13.5" thickTop="1">
+    <row r="18" spans="1:23" ht="13.2" thickTop="1">
       <c r="A18" s="205"/>
       <c r="B18" s="152">
         <v>7</v>
@@ -56857,7 +56857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="13.5" thickBot="1">
+    <row r="29" spans="1:23" ht="13.2" thickBot="1">
       <c r="A29" s="205"/>
       <c r="B29" s="156">
         <v>26</v>
@@ -56926,7 +56926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="13.5" thickTop="1">
+    <row r="30" spans="1:23" ht="13.2" thickTop="1">
       <c r="A30" s="205"/>
       <c r="B30" s="114">
         <v>28</v>
@@ -57088,7 +57088,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="198" t="s">
@@ -57119,7 +57119,7 @@
       <c r="V1" s="199"/>
       <c r="W1" s="199"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1">
+    <row r="2" spans="1:23" ht="15" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="48" t="s">
         <v>87</v>
@@ -59487,7 +59487,7 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
   </cols>
@@ -59521,7 +59521,7 @@
       <c r="V1" s="199"/>
       <c r="W1" s="199"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1">
+    <row r="2" spans="1:23" ht="15" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="48" t="s">
         <v>86</v>
@@ -61890,7 +61890,7 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="206" t="s">
@@ -61921,7 +61921,7 @@
       <c r="V1" s="207"/>
       <c r="W1" s="207"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1">
+    <row r="2" spans="1:23" ht="15" thickBot="1">
       <c r="A2" s="206"/>
       <c r="B2" s="128" t="s">
         <v>88</v>
@@ -64290,9 +64290,9 @@
       <selection activeCell="B2" sqref="B2:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -64750,9 +64750,9 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:9" s="126" customFormat="1" ht="60">
+    <row r="1" spans="1:9" s="126" customFormat="1" ht="43.2">
       <c r="A1" s="125" t="s">
         <v>80</v>
       </c>
@@ -66059,11 +66059,11 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="22" width="5.7109375" customWidth="1"/>
-    <col min="23" max="23" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="22" width="5.6640625" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -68322,11 +68322,11 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="99" customWidth="1"/>
-    <col min="3" max="23" width="6.85546875" style="104" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" style="99" customWidth="1"/>
+    <col min="3" max="23" width="6.88671875" style="104" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -68354,7 +68354,7 @@
       <c r="V1" s="197"/>
       <c r="W1" s="197"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1">
+    <row r="2" spans="1:23" ht="15" thickBot="1">
       <c r="B2" s="105" t="s">
         <v>35</v>
       </c>
@@ -70586,14 +70586,14 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="95" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="95" customWidth="1"/>
     <col min="4" max="4" width="11" style="95" customWidth="1"/>
-    <col min="5" max="22" width="8.140625" style="95" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" style="95" customWidth="1"/>
+    <col min="5" max="22" width="8.109375" style="95" customWidth="1"/>
+    <col min="23" max="23" width="13.33203125" style="95" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -72855,10 +72855,10 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -72867,7 +72867,7 @@
     <col min="18" max="18" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="22" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.42578125" style="3"/>
+    <col min="24" max="16384" width="5.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -72900,7 +72900,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.5" thickBot="1">
+    <row r="2" spans="1:24" ht="13.2" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="71" t="s">
         <v>7</v>
@@ -74992,7 +74992,7 @@
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="200" t="s">
@@ -75023,7 +75023,7 @@
       <c r="V1" s="201"/>
       <c r="W1" s="201"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1">
+    <row r="2" spans="1:23" ht="15" thickBot="1">
       <c r="A2" s="200"/>
       <c r="B2" s="190" t="s">
         <v>87</v>
@@ -77386,7 +77386,7 @@
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="200" t="s">
@@ -77417,7 +77417,7 @@
       <c r="V1" s="201"/>
       <c r="W1" s="201"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1">
+    <row r="2" spans="1:23" ht="15" thickBot="1">
       <c r="A2" s="200"/>
       <c r="B2" s="190" t="s">
         <v>87</v>

</xml_diff>